<commit_message>
cambio en el código del main.js porque no funcionaba la fecha y y la cantActual del inventario
</commit_message>
<xml_diff>
--- a/data/inventario_minsal.xlsx
+++ b/data/inventario_minsal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C826D6DD-5A66-4CE8-9A5F-E507BD5BDBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D6CA8B9-F898-4003-86A1-DF571CFEA736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{33EF6376-3F5A-46D1-9B87-DA96CC38AB62}"/>
+    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8880" xr2:uid="{33EF6376-3F5A-46D1-9B87-DA96CC38AB62}"/>
   </bookViews>
   <sheets>
     <sheet name="Catálogo" sheetId="1" r:id="rId1"/>
@@ -396,7 +396,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,6 +430,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -483,7 +491,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -548,6 +556,8 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -863,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275FD917-88A1-4BCB-B444-9B25C23BB9C3}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1142,6 +1152,12 @@
       <c r="I9" s="1" t="s">
         <v>70</v>
       </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="26"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F19" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1699,7 +1715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE35B441-4330-4DE7-BF4C-33686CF5BC29}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -1977,7 +1993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14699FA6-5CB9-438C-BC81-74BB6D2876AB}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="C7" zoomScale="75" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
agrego modulos de compra y salida, aun faltan mejorar varias funciones
</commit_message>
<xml_diff>
--- a/data/inventario_minsal.xlsx
+++ b/data/inventario_minsal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sistema_inventariosMinsal\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D6CA8B9-F898-4003-86A1-DF571CFEA736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E97531F-1BD5-4B80-8C1B-E685F3F01D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8880" xr2:uid="{33EF6376-3F5A-46D1-9B87-DA96CC38AB62}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{33EF6376-3F5A-46D1-9B87-DA96CC38AB62}"/>
   </bookViews>
   <sheets>
     <sheet name="Catálogo" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="119">
   <si>
     <t>Código</t>
   </si>
@@ -262,9 +262,6 @@
     <t>10mg</t>
   </si>
   <si>
-    <t>=SUMAR.SI(Inventario_Lotes!B:B,A8,Inventario_Lotes!F:F)</t>
-  </si>
-  <si>
     <t>MED-008</t>
   </si>
   <si>
@@ -274,9 +271,6 @@
     <t>400mg</t>
   </si>
   <si>
-    <t>=SUMAR.SI(Inventario_Lotes!B:B,A9,Inventario_Lotes!F:F)</t>
-  </si>
-  <si>
     <t>L001</t>
   </si>
   <si>
@@ -295,9 +289,6 @@
     <t xml:space="preserve"> LOT-2025-023 </t>
   </si>
   <si>
-    <t xml:space="preserve"> 10/06/2025 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> L003 </t>
   </si>
   <si>
@@ -373,9 +364,6 @@
     <t>🔴 ¡ALERTA! PRÓXIMOS A VENCER</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Clase_Abc</t>
   </si>
   <si>
@@ -386,6 +374,51 @@
   </si>
   <si>
     <t xml:space="preserve"> LOT-2025-089</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> L006</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> L007</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> L008</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LOT-2025-090</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LOT-2025-091</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LOT-2025-092</t>
+  </si>
+  <si>
+    <t>MED-009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aspirina </t>
+  </si>
+  <si>
+    <t>100 mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LOT-2025-093</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F-001237</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F-001238</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F-001239</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F-001240</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F-001241</t>
   </si>
 </sst>
 </file>
@@ -491,7 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -557,7 +590,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -873,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275FD917-88A1-4BCB-B444-9B25C23BB9C3}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,7 +1003,7 @@
         <v>50000</v>
       </c>
       <c r="I3" s="1">
-        <f>SUMIF(Inventario_Lotes!B:B,A3,Inventario_Lotes!F:F)</f>
+        <f>SUMIF(Inventario_Lotes!B:B,TRIM(A3),Inventario_Lotes!F:F)</f>
         <v>300</v>
       </c>
     </row>
@@ -1001,7 +1033,7 @@
         <v>10000</v>
       </c>
       <c r="I4" s="1">
-        <f>SUMIF(Inventario_Lotes!B:B,A4,Inventario_Lotes!F:F)</f>
+        <f>SUMIF(Inventario_Lotes!B:B,TRIM(A4),Inventario_Lotes!F:F)</f>
         <v>9210</v>
       </c>
     </row>
@@ -1031,7 +1063,7 @@
         <v>20000</v>
       </c>
       <c r="I5" s="1">
-        <f>SUMIF(Inventario_Lotes!B:B,A5,Inventario_Lotes!F:F)</f>
+        <f>SUMIF(Inventario_Lotes!B:B,TRIM(A5),Inventario_Lotes!F:F)</f>
         <v>9300</v>
       </c>
     </row>
@@ -1061,7 +1093,7 @@
         <v>30000</v>
       </c>
       <c r="I6" s="1">
-        <f>SUMIF(Inventario_Lotes!B:B,A6,Inventario_Lotes!F:F)</f>
+        <f>SUMIF(Inventario_Lotes!B:B,TRIM(A6),Inventario_Lotes!F:F)</f>
         <v>10000</v>
       </c>
     </row>
@@ -1091,11 +1123,11 @@
         <v>40000</v>
       </c>
       <c r="I7" s="1">
-        <f>SUMIF(Inventario_Lotes!B:B,A7,Inventario_Lotes!F:F)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <f>SUMIF(Inventario_Lotes!B:B,TRIM(A7),Inventario_Lotes!F:F)</f>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>63</v>
       </c>
@@ -1120,22 +1152,23 @@
       <c r="H8" s="1">
         <v>35000</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="1">
+        <f>SUMIF(Inventario_Lotes!B:B,TRIM(A8),Inventario_Lotes!F:F)</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="3">
         <v>0.03</v>
@@ -1149,27 +1182,52 @@
       <c r="H9" s="1">
         <v>25000</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>70</v>
+      <c r="I9" s="1">
+        <f>SUMIF(Inventario_Lotes!B:B,TRIM(A9),Inventario_Lotes!F:F)</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H10" s="1">
+        <v>5000</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I13" s="26"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F19" s="27"/>
-    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCCC6A64-6EEC-4F9D-92CD-772FEB3A9BD0}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1222,7 +1280,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>40</v>
@@ -1232,7 +1290,7 @@
         <v>Insulina NPH</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E2" s="10">
         <v>1000</v>
@@ -1250,13 +1308,13 @@
         <v>55</v>
       </c>
       <c r="J2" s="1" t="str">
-        <f ca="1">IF(F2&lt;=0,"❌ Agotado",IF((H2-TODAY())&lt;=30,"⚠️ Por Vencer","✅ Activo"))</f>
+        <f t="shared" ref="J2:J9" ca="1" si="0">IF(F2&lt;=0,"❌ Agotado",IF((H2-TODAY())&lt;=30,"⚠️ Por Vencer","✅ Activo"))</f>
         <v>⚠️ Por Vencer</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="115.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>45</v>
@@ -1266,7 +1324,7 @@
         <v>Paracetamol</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E3" s="10">
         <v>500</v>
@@ -1274,8 +1332,8 @@
       <c r="F3" s="10">
         <v>300</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>75</v>
+      <c r="G3" s="8">
+        <v>45919</v>
       </c>
       <c r="H3" s="8">
         <v>46614</v>
@@ -1284,13 +1342,13 @@
         <v>45</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f ca="1">IF(F3&lt;=0,"❌ Agotado",IF((H3-TODAY())&lt;=30,"⚠️ Por Vencer","✅ Activo"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>✅ Activo</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>50</v>
@@ -1300,7 +1358,7 @@
         <v>Amoxicilina</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E4" s="10">
         <v>50000</v>
@@ -1308,8 +1366,8 @@
       <c r="F4" s="10">
         <v>9210</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>77</v>
+      <c r="G4" s="8">
+        <v>45697</v>
       </c>
       <c r="H4" s="8">
         <v>46548</v>
@@ -1318,13 +1376,13 @@
         <v>0.12</v>
       </c>
       <c r="J4" s="1" t="str">
-        <f ca="1">IF(F4&lt;=0,"❌ Agotado",IF((H4-TODAY())&lt;=30,"⚠️ Por Vencer","✅ Activo"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>✅ Activo</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="121.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>54</v>
@@ -1334,7 +1392,7 @@
         <v>Omeprazol</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E5" s="10">
         <v>10000</v>
@@ -1342,23 +1400,23 @@
       <c r="F5" s="10">
         <v>9300</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>81</v>
+      <c r="G5" s="8">
+        <v>45912</v>
       </c>
       <c r="H5" s="21">
-        <v>46278</v>
+        <v>47190</v>
       </c>
       <c r="I5" s="11">
         <v>0.85</v>
       </c>
       <c r="J5" s="1" t="str">
-        <f ca="1">IF(F5&lt;=0,"❌ Agotado",IF((H5-TODAY())&lt;=30,"⚠️ Por Vencer","✅ Activo"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>✅ Activo</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>57</v>
@@ -1368,7 +1426,7 @@
         <v>Losartán</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E6" s="10">
         <v>8000</v>
@@ -1377,7 +1435,7 @@
         <v>10000</v>
       </c>
       <c r="G6" s="8">
-        <v>45941</v>
+        <v>45576</v>
       </c>
       <c r="H6" s="8">
         <v>45971</v>
@@ -1386,8 +1444,115 @@
         <v>1</v>
       </c>
       <c r="J6" s="10" t="str">
-        <f ca="1">IF(F6&lt;=0,"❌ Agotado",IF((H6-TODAY())&lt;=30,"⚠️ Por Vencer","✅ Activo"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>⚠️ Por Vencer</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="10" t="str">
+        <f>VLOOKUP(B7,Catálogo!A:B,2,0)</f>
+        <v>Metformina</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="10">
+        <v>10000</v>
+      </c>
+      <c r="F7" s="10">
+        <v>25000</v>
+      </c>
+      <c r="G7" s="8">
+        <v>45239</v>
+      </c>
+      <c r="H7" s="8">
+        <v>46023</v>
+      </c>
+      <c r="I7" s="11">
+        <v>2</v>
+      </c>
+      <c r="J7" s="10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>✅ Activo</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="10" t="str">
+        <f>VLOOKUP(B8,Catálogo!A:B,2,0)</f>
+        <v>Enalapril</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="10">
+        <v>8000</v>
+      </c>
+      <c r="F8" s="10">
+        <v>15000</v>
+      </c>
+      <c r="G8" s="8">
+        <v>45292</v>
+      </c>
+      <c r="H8" s="8">
+        <v>46022</v>
+      </c>
+      <c r="I8" s="11">
+        <v>5</v>
+      </c>
+      <c r="J8" s="10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>✅ Activo</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="10" t="str">
+        <f>VLOOKUP(B9,Catálogo!A:B,2,0)</f>
+        <v>Ibuprofeno</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="10">
+        <v>5000</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1200</v>
+      </c>
+      <c r="G9" s="8">
+        <v>45595</v>
+      </c>
+      <c r="H9" s="8">
+        <v>47062</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="J9" s="10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>✅ Activo</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D10" s="10" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1398,10 +1563,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2DD2F9-1CC9-4744-AF0B-6F5BCD540E28}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1435,7 +1600,7 @@
         <v>22</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>12</v>
@@ -1461,10 +1626,10 @@
         <v>45884</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>40</v>
@@ -1478,7 +1643,7 @@
         <v>A</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H2" s="6">
         <v>1000</v>
@@ -1502,13 +1667,13 @@
     </row>
     <row r="3" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>45</v>
@@ -1522,7 +1687,7 @@
         <v>C</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H3" s="14">
         <v>200</v>
@@ -1546,13 +1711,13 @@
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>50</v>
@@ -1566,7 +1731,7 @@
         <v>B</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H4" s="14">
         <v>100</v>
@@ -1589,31 +1754,153 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="D5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="6" t="str">
+        <f>IFERROR(VLOOKUP(TRIM(D5),Catálogo!A:B,2,FALSE),"❌ No encontrado")</f>
+        <v>Omeprazol</v>
+      </c>
+      <c r="F5" s="7" t="str">
+        <f>IFERROR(VLOOKUP(TRIM(D5),Catálogo!A:F,6,FALSE),"")</f>
+        <v>A</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>103</v>
       </c>
+      <c r="I5" s="13">
+        <f>IFERROR(VLOOKUP(TRIM(D5),Catálogo!A:E,5,FALSE),"")</f>
+        <v>0.12</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="D6" s="7" t="s">
-        <v>103</v>
+        <v>57</v>
+      </c>
+      <c r="E6" s="6" t="str">
+        <f>IFERROR(VLOOKUP(TRIM(D6),Catálogo!A:B,2,FALSE),"❌ No encontrado")</f>
+        <v>Losartán</v>
+      </c>
+      <c r="F6" s="7" t="str">
+        <f>IFERROR(VLOOKUP(TRIM(D6),Catálogo!A:F,6,FALSE),"")</f>
+        <v>A</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" s="13">
+        <f>IFERROR(VLOOKUP(TRIM(D6),Catálogo!A:E,5,FALSE),"")</f>
+        <v>0.08</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="D7" s="7" t="s">
-        <v>103</v>
+        <v>60</v>
+      </c>
+      <c r="E7" s="6" t="str">
+        <f>IFERROR(VLOOKUP(TRIM(D7),Catálogo!A:B,2,FALSE),"❌ No encontrado")</f>
+        <v>Metformina</v>
+      </c>
+      <c r="F7" s="7" t="str">
+        <f>IFERROR(VLOOKUP(TRIM(D7),Catálogo!A:F,6,FALSE),"")</f>
+        <v>A</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="13">
+        <f>IFERROR(VLOOKUP(TRIM(D7),Catálogo!A:E,5,FALSE),"")</f>
+        <v>0.06</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="D8" s="7" t="s">
-        <v>103</v>
+        <v>63</v>
+      </c>
+      <c r="E8" s="6" t="str">
+        <f>IFERROR(VLOOKUP(TRIM(D8),Catálogo!A:B,2,FALSE),"❌ No encontrado")</f>
+        <v>Enalapril</v>
+      </c>
+      <c r="F8" s="7" t="str">
+        <f>IFERROR(VLOOKUP(TRIM(D8),Catálogo!A:F,6,FALSE),"")</f>
+        <v>A</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="13">
+        <f>IFERROR(VLOOKUP(TRIM(D8),Catálogo!A:E,5,FALSE),"")</f>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="6" t="str">
+        <f>IFERROR(VLOOKUP(TRIM(D9),Catálogo!A:B,2,FALSE),"❌ No encontrado")</f>
+        <v>Ibuprofeno</v>
+      </c>
+      <c r="F9" s="7" t="str">
+        <f>IFERROR(VLOOKUP(TRIM(D9),Catálogo!A:F,6,FALSE),"")</f>
+        <v>B</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" s="13">
+        <f>IFERROR(VLOOKUP(TRIM(D9),Catálogo!A:E,5,FALSE),"")</f>
+        <v>0.03</v>
+      </c>
       <c r="J9" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D10" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="6" t="str">
+        <f>IFERROR(VLOOKUP(TRIM(D10),Catálogo!A:B,2,FALSE),"❌ No encontrado")</f>
+        <v xml:space="preserve">Aspirina </v>
+      </c>
+      <c r="I10" s="13">
+        <f>IFERROR(VLOOKUP(TRIM(D10),Catálogo!A:E,5,FALSE),"")</f>
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1676,10 +1963,10 @@
         <v>45889</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>40</v>
@@ -1689,7 +1976,7 @@
         <v>Insulina NPH</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G2" s="6">
         <v>150</v>
@@ -1703,7 +1990,7 @@
         <v>8250</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1756,16 +2043,16 @@
     <row r="2" spans="1:7" s="19" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
@@ -1787,10 +2074,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
         <v>92</v>
-      </c>
-      <c r="D4" t="s">
-        <v>95</v>
       </c>
       <c r="E4" t="s">
         <v>40</v>
@@ -1800,21 +2087,21 @@
         <v>5200</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E5" t="s">
         <v>40</v>
@@ -1826,16 +2113,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B10" s="7">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E10" t="s">
         <v>40</v>
@@ -1847,16 +2134,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B11" s="5">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E11" t="s">
         <v>40</v>
@@ -1905,12 +2192,12 @@
         <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1977,7 +2264,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F7" s="25" cm="1">
         <f t="array" ref="F7">LOOKUP(2,1/(VALUE(F3:F6)&lt;&gt;0),VALUE(F3:F6))</f>
@@ -1991,10 +2278,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14699FA6-5CB9-438C-BC81-74BB6D2876AB}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="C40" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2026,7 +2313,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" t="str" cm="1">
         <f t="array" ref="B2">IF(INDEX(Catálogo!I:I,ROW(A2))&lt;INDEX(Catálogo!G:G,ROW(A2)),INDEX(Catálogo!A:A,ROW(A2)),"")</f>
@@ -2047,7 +2334,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B3" t="str" cm="1">
         <f t="array" ref="B3">IF(INDEX(Catálogo!I:I,ROW(A3))&lt;INDEX(Catálogo!G:G,ROW(A3)),INDEX(Catálogo!A:A,ROW(A3)),"")</f>
@@ -2068,7 +2355,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B4" t="str" cm="1">
         <f t="array" ref="B4">IF(INDEX(Catálogo!I:I,ROW(A4))&lt;INDEX(Catálogo!G:G,ROW(A4)),INDEX(Catálogo!A:A,ROW(A4)),"")</f>
@@ -2089,7 +2376,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B5" t="str" cm="1">
         <f t="array" ref="B5">IF(INDEX(Catálogo!I:I,ROW(A5))&lt;INDEX(Catálogo!G:G,ROW(A5)),INDEX(Catálogo!A:A,ROW(A5)),"")</f>
@@ -2110,7 +2397,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B6" t="str" cm="1">
         <f t="array" ref="B6">IF(INDEX(Catálogo!I:I,ROW(A6))&lt;INDEX(Catálogo!G:G,ROW(A6)),INDEX(Catálogo!A:A,ROW(A6)),"")</f>
@@ -2131,15 +2418,15 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B7" t="str" cm="1">
         <f t="array" ref="B7">IF(INDEX(Catálogo!I:I,ROW(A7))&lt;INDEX(Catálogo!G:G,ROW(A7)),INDEX(Catálogo!A:A,ROW(A7)),"")</f>
-        <v>MED-006</v>
+        <v/>
       </c>
       <c r="C7" t="str">
         <f>IF(B7&lt;&gt;"",VLOOKUP(B7,Catálogo!A:B,2,FALSE),"")</f>
-        <v>Metformina</v>
+        <v/>
       </c>
       <c r="D7" t="str">
         <f>IF(B6&lt;&gt;"","Stock actual: "&amp;VLOOKUP(B6,Catálogo!A:I,9,FALSE)&amp;" | Mínimo: "&amp;VLOOKUP(B6,Catálogo!A:G,7,FALSE),"")</f>
@@ -2147,12 +2434,12 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>🛒 COMPRAR URGENTE</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B8" t="str" cm="1">
         <f t="array" ref="B8">IF(INDEX(Catálogo!I:I,ROW(A8))&lt;INDEX(Catálogo!G:G,ROW(A8)),INDEX(Catálogo!A:A,ROW(A8)),"")</f>
@@ -2164,7 +2451,7 @@
       </c>
       <c r="D8" t="str">
         <f>IF(B7&lt;&gt;"","Stock actual: "&amp;VLOOKUP(B7,Catálogo!A:I,9,FALSE)&amp;" | Mínimo: "&amp;VLOOKUP(B7,Catálogo!A:G,7,FALSE),"")</f>
-        <v>Stock actual: 0 | Mínimo: 10000</v>
+        <v/>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -2173,15 +2460,15 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B9" t="str" cm="1">
         <f t="array" ref="B9">IF(INDEX(Catálogo!I:I,ROW(A9))&lt;INDEX(Catálogo!G:G,ROW(A9)),INDEX(Catálogo!A:A,ROW(A9)),"")</f>
-        <v/>
+        <v>MED-008</v>
       </c>
       <c r="C9" t="str">
         <f>IF(B9&lt;&gt;"",VLOOKUP(B9,Catálogo!A:B,2,FALSE),"")</f>
-        <v/>
+        <v>Ibuprofeno</v>
       </c>
       <c r="D9" t="str">
         <f>IF(B8&lt;&gt;"","Stock actual: "&amp;VLOOKUP(B8,Catálogo!A:I,9,FALSE)&amp;" | Mínimo: "&amp;VLOOKUP(B8,Catálogo!A:G,7,FALSE),"")</f>
@@ -2189,33 +2476,33 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>🛒 COMPRAR URGENTE</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10">IF(INDEX(Catálogo!I:I,ROW(A10))&lt;INDEX(Catálogo!G:G,ROW(A10)),INDEX(Catálogo!A:A,ROW(A10)),"")</f>
-        <v/>
+        <v>MED-009</v>
       </c>
       <c r="C10" t="str">
         <f>IF(B10&lt;&gt;"",VLOOKUP(B10,Catálogo!A:B,2,FALSE),"")</f>
-        <v/>
+        <v xml:space="preserve">Aspirina </v>
       </c>
       <c r="D10" t="str">
         <f>IF(B9&lt;&gt;"","Stock actual: "&amp;VLOOKUP(B9,Catálogo!A:I,9,FALSE)&amp;" | Mínimo: "&amp;VLOOKUP(B9,Catálogo!A:G,7,FALSE),"")</f>
-        <v/>
+        <v>Stock actual: 1200 | Mínimo: 5000</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>🛒 COMPRAR URGENTE</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B11" t="str" cm="1">
         <f t="array" ref="B11">IF(INDEX(Catálogo!I:I,ROW(A11))&lt;INDEX(Catálogo!G:G,ROW(A11)),INDEX(Catálogo!A:A,ROW(A11)),"")</f>
@@ -2227,7 +2514,7 @@
       </c>
       <c r="D11" t="str">
         <f>IF(B10&lt;&gt;"","Stock actual: "&amp;VLOOKUP(B10,Catálogo!A:I,9,FALSE)&amp;" | Mínimo: "&amp;VLOOKUP(B10,Catálogo!A:G,7,FALSE),"")</f>
-        <v/>
+        <v>Stock actual:  | Mínimo: 1000</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -2236,7 +2523,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B12" t="str" cm="1">
         <f t="array" ref="B12">IF(INDEX(Catálogo!I:I,ROW(A12))&lt;INDEX(Catálogo!G:G,ROW(A12)),INDEX(Catálogo!A:A,ROW(A12)),"")</f>
@@ -2257,7 +2544,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B13" t="str" cm="1">
         <f t="array" ref="B13">IF(INDEX(Catálogo!I:I,ROW(A13))&lt;INDEX(Catálogo!G:G,ROW(A13)),INDEX(Catálogo!A:A,ROW(A13)),"")</f>
@@ -2278,7 +2565,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B14" t="str" cm="1">
         <f t="array" ref="B14">IF(INDEX(Catálogo!I:I,ROW(A14))&lt;INDEX(Catálogo!G:G,ROW(A14)),INDEX(Catálogo!A:A,ROW(A14)),"")</f>
@@ -2299,7 +2586,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B15" t="str" cm="1">
         <f t="array" ref="B15">IF(INDEX(Catálogo!I:I,ROW(A15))&lt;INDEX(Catálogo!G:G,ROW(A15)),INDEX(Catálogo!A:A,ROW(A15)),"")</f>
@@ -2320,7 +2607,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B16" t="str" cm="1">
         <f t="array" ref="B16">IF(INDEX(Catálogo!I:I,ROW(A16))&lt;INDEX(Catálogo!G:G,ROW(A16)),INDEX(Catálogo!A:A,ROW(A16)),"")</f>
@@ -2341,7 +2628,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B17" t="str" cm="1">
         <f t="array" ref="B17">IF(INDEX(Catálogo!I:I,ROW(A17))&lt;INDEX(Catálogo!G:G,ROW(A17)),INDEX(Catálogo!A:A,ROW(A17)),"")</f>
@@ -2362,7 +2649,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B18" t="str" cm="1">
         <f t="array" ref="B18">IF(INDEX(Catálogo!I:I,ROW(A18))&lt;INDEX(Catálogo!G:G,ROW(A18)),INDEX(Catálogo!A:A,ROW(A18)),"")</f>
@@ -2383,7 +2670,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B19" t="str" cm="1">
         <f t="array" ref="B19">IF(INDEX(Catálogo!I:I,ROW(A19))&lt;INDEX(Catálogo!G:G,ROW(A19)),INDEX(Catálogo!A:A,ROW(A19)),"")</f>
@@ -2404,7 +2691,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B20" t="str" cm="1">
         <f t="array" ref="B20">IF(INDEX(Catálogo!I:I,ROW(A20))&lt;INDEX(Catálogo!G:G,ROW(A20)),INDEX(Catálogo!A:A,ROW(A20)),"")</f>
@@ -2425,7 +2712,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B21" t="str" cm="1">
         <f t="array" ref="B21">IF(INDEX(Catálogo!I:I,ROW(A21))&lt;INDEX(Catálogo!G:G,ROW(A21)),INDEX(Catálogo!A:A,ROW(A21)),"")</f>
@@ -2446,7 +2733,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B22" t="str" cm="1">
         <f t="array" ref="B22">IF(INDEX(Catálogo!I:I,ROW(A22))&lt;INDEX(Catálogo!G:G,ROW(A22)),INDEX(Catálogo!A:A,ROW(A22)),"")</f>
@@ -2467,7 +2754,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B23" t="str" cm="1">
         <f t="array" ref="B23">IF(INDEX(Catálogo!I:I,ROW(A23))&lt;INDEX(Catálogo!G:G,ROW(A23)),INDEX(Catálogo!A:A,ROW(A23)),"")</f>
@@ -2488,7 +2775,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B24" t="str" cm="1">
         <f t="array" ref="B24">IF(INDEX(Catálogo!I:I,ROW(A24))&lt;INDEX(Catálogo!G:G,ROW(A24)),INDEX(Catálogo!A:A,ROW(A24)),"")</f>
@@ -2509,7 +2796,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B25" t="str" cm="1">
         <f t="array" ref="B25">IF(INDEX(Catálogo!I:I,ROW(A25))&lt;INDEX(Catálogo!G:G,ROW(A25)),INDEX(Catálogo!A:A,ROW(A25)),"")</f>
@@ -2530,7 +2817,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B26" t="str" cm="1">
         <f t="array" ref="B26">IF(INDEX(Catálogo!I:I,ROW(A26))&lt;INDEX(Catálogo!G:G,ROW(A26)),INDEX(Catálogo!A:A,ROW(A26)),"")</f>
@@ -2551,7 +2838,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B27" t="str" cm="1">
         <f t="array" ref="B27">IF(INDEX(Catálogo!I:I,ROW(A27))&lt;INDEX(Catálogo!G:G,ROW(A27)),INDEX(Catálogo!A:A,ROW(A27)),"")</f>
@@ -2572,7 +2859,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B28" t="str" cm="1">
         <f t="array" ref="B28">IF(INDEX(Catálogo!I:I,ROW(A28))&lt;INDEX(Catálogo!G:G,ROW(A28)),INDEX(Catálogo!A:A,ROW(A28)),"")</f>
@@ -2593,7 +2880,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B29" t="str" cm="1">
         <f t="array" ref="B29">IF(INDEX(Catálogo!I:I,ROW(A29))&lt;INDEX(Catálogo!G:G,ROW(A29)),INDEX(Catálogo!A:A,ROW(A29)),"")</f>
@@ -2614,7 +2901,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B30" t="str" cm="1">
         <f t="array" ref="B30">IF(INDEX(Catálogo!I:I,ROW(A30))&lt;INDEX(Catálogo!G:G,ROW(A30)),INDEX(Catálogo!A:A,ROW(A30)),"")</f>
@@ -2635,7 +2922,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B31" t="str" cm="1">
         <f t="array" ref="B31">IF(INDEX(Catálogo!I:I,ROW(A31))&lt;INDEX(Catálogo!G:G,ROW(A31)),INDEX(Catálogo!A:A,ROW(A31)),"")</f>
@@ -2657,7 +2944,7 @@
     <row r="35" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B36" t="str">
         <f ca="1">IF((Inventario_Lotes!H2-TODAY())&lt;=30,Inventario_Lotes!D2,"")</f>
@@ -2669,7 +2956,7 @@
       </c>
       <c r="D36" t="str">
         <f ca="1">IF(B36&lt;&gt;"","Lote vence el "&amp;TEXT(VLOOKUP(B36,Inventario_Lotes!D:H,5,FALSE),"dd/mm/aaaa")&amp;" ("&amp;ROUND((VLOOKUP(B36,Inventario_Lotes!D:H,5,FALSE)-TODAY()),0)&amp;" días)","")</f>
-        <v>Lote vence el 01/08/jueves (-448 días)</v>
+        <v>Lote vence el 01/08/jueves (-450 días)</v>
       </c>
       <c r="E36" t="str">
         <f ca="1">IF(B36&lt;&gt;"","⚠️ USAR PRIORITARIAMENTE","")</f>
@@ -2678,7 +2965,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B37" t="str">
         <f ca="1">IF((Inventario_Lotes!H3-TODAY())&lt;=30,Inventario_Lotes!D3,"")</f>
@@ -2699,7 +2986,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B38" t="str">
         <f ca="1">IF((Inventario_Lotes!H4-TODAY())&lt;=30,Inventario_Lotes!D4,"")</f>
@@ -2720,7 +3007,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B39" t="str">
         <f ca="1">IF((Inventario_Lotes!H5-TODAY())&lt;=30,Inventario_Lotes!D5,"")</f>
@@ -2741,7 +3028,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B40" t="str">
         <f ca="1">IF((Inventario_Lotes!H6-TODAY())&lt;=30,Inventario_Lotes!D6,"")</f>
@@ -2753,7 +3040,7 @@
       </c>
       <c r="D40" t="str">
         <f ca="1">IF(B40&lt;&gt;"","Lote vence el "&amp;TEXT(VLOOKUP(B40,Inventario_Lotes!D:H,5,FALSE),"dd/mm/aaaa")&amp;" ("&amp;ROUND((VLOOKUP(B40,Inventario_Lotes!D:H,5,FALSE)-TODAY()),0)&amp;" días)","")</f>
-        <v>Lote vence el 10/11/lunes (18 días)</v>
+        <v>Lote vence el 10/11/lunes (16 días)</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2762,82 +3049,82 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B41">
+        <v>99</v>
+      </c>
+      <c r="B41" t="str">
         <f ca="1">IF((Inventario_Lotes!H7-TODAY())&lt;=30,Inventario_Lotes!D7,"")</f>
-        <v>0</v>
-      </c>
-      <c r="C41" t="e">
+        <v/>
+      </c>
+      <c r="C41" t="str">
         <f ca="1">IF(B41&lt;&gt;"",INDEX(Inventario_Lotes!C:C,MATCH(B41,Inventario_Lotes!D:D,0)),"")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D41" t="e">
+        <v/>
+      </c>
+      <c r="D41" t="str">
         <f ca="1">IF(B41&lt;&gt;"","Lote vence el "&amp;TEXT(VLOOKUP(B41,Inventario_Lotes!D:H,5,FALSE),"dd/mm/aaaa")&amp;" ("&amp;ROUND((VLOOKUP(B41,Inventario_Lotes!D:H,5,FALSE)-TODAY()),0)&amp;" días)","")</f>
-        <v>#N/A</v>
+        <v/>
       </c>
       <c r="E41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>⚠️ USAR PRIORITARIAMENTE</v>
+        <v/>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42">
+        <v>99</v>
+      </c>
+      <c r="B42" t="str">
         <f ca="1">IF((Inventario_Lotes!H8-TODAY())&lt;=30,Inventario_Lotes!D8,"")</f>
-        <v>0</v>
-      </c>
-      <c r="C42" t="e">
+        <v/>
+      </c>
+      <c r="C42" t="str">
         <f ca="1">IF(B42&lt;&gt;"",INDEX(Inventario_Lotes!C:C,MATCH(B42,Inventario_Lotes!D:D,0)),"")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D42" t="e">
+        <v/>
+      </c>
+      <c r="D42" t="str">
         <f ca="1">IF(B42&lt;&gt;"","Lote vence el "&amp;TEXT(VLOOKUP(B42,Inventario_Lotes!D:H,5,FALSE),"dd/mm/aaaa")&amp;" ("&amp;ROUND((VLOOKUP(B42,Inventario_Lotes!D:H,5,FALSE)-TODAY()),0)&amp;" días)","")</f>
-        <v>#N/A</v>
+        <v/>
       </c>
       <c r="E42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>⚠️ USAR PRIORITARIAMENTE</v>
+        <v/>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B43">
+        <v>99</v>
+      </c>
+      <c r="B43" t="str">
         <f ca="1">IF((Inventario_Lotes!H9-TODAY())&lt;=30,Inventario_Lotes!D9,"")</f>
-        <v>0</v>
-      </c>
-      <c r="C43" t="e">
+        <v/>
+      </c>
+      <c r="C43" t="str">
         <f ca="1">IF(B43&lt;&gt;"",INDEX(Inventario_Lotes!C:C,MATCH(B43,Inventario_Lotes!D:D,0)),"")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D43" t="e">
+        <v/>
+      </c>
+      <c r="D43" t="str">
         <f ca="1">IF(B43&lt;&gt;"","Lote vence el "&amp;TEXT(VLOOKUP(B43,Inventario_Lotes!D:H,5,FALSE),"dd/mm/aaaa")&amp;" ("&amp;ROUND((VLOOKUP(B43,Inventario_Lotes!D:H,5,FALSE)-TODAY()),0)&amp;" días)","")</f>
-        <v>#N/A</v>
+        <v/>
       </c>
       <c r="E43" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>⚠️ USAR PRIORITARIAMENTE</v>
+        <v/>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B44">
+        <v>99</v>
+      </c>
+      <c r="B44" t="str">
         <f ca="1">IF((Inventario_Lotes!H10-TODAY())&lt;=30,Inventario_Lotes!D10,"")</f>
+        <v xml:space="preserve"> LOT-2025-093</v>
+      </c>
+      <c r="C44">
+        <f ca="1">IF(B44&lt;&gt;"",INDEX(Inventario_Lotes!C:C,MATCH(B44,Inventario_Lotes!D:D,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="C44" t="e">
-        <f ca="1">IF(B44&lt;&gt;"",INDEX(Inventario_Lotes!C:C,MATCH(B44,Inventario_Lotes!D:D,0)),"")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D44" t="e">
+      <c r="D44" t="str">
         <f ca="1">IF(B44&lt;&gt;"","Lote vence el "&amp;TEXT(VLOOKUP(B44,Inventario_Lotes!D:H,5,FALSE),"dd/mm/aaaa")&amp;" ("&amp;ROUND((VLOOKUP(B44,Inventario_Lotes!D:H,5,FALSE)-TODAY()),0)&amp;" días)","")</f>
-        <v>#N/A</v>
+        <v>Lote vence el 00/01/sábado (-45955 días)</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2846,7 +3133,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B45">
         <f ca="1">IF((Inventario_Lotes!H11-TODAY())&lt;=30,Inventario_Lotes!D11,"")</f>
@@ -2867,7 +3154,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B46">
         <f ca="1">IF((Inventario_Lotes!H12-TODAY())&lt;=30,Inventario_Lotes!D12,"")</f>
@@ -2888,7 +3175,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B47">
         <f ca="1">IF((Inventario_Lotes!H13-TODAY())&lt;=30,Inventario_Lotes!D13,"")</f>
@@ -2909,7 +3196,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B48">
         <f ca="1">IF((Inventario_Lotes!H14-TODAY())&lt;=30,Inventario_Lotes!D14,"")</f>
@@ -2930,7 +3217,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B49">
         <f ca="1">IF((Inventario_Lotes!H15-TODAY())&lt;=30,Inventario_Lotes!D15,"")</f>
@@ -2951,7 +3238,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B50">
         <f ca="1">IF((Inventario_Lotes!H16-TODAY())&lt;=30,Inventario_Lotes!D16,"")</f>
@@ -2968,6 +3255,12 @@
       <c r="E50" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>⚠️ USAR PRIORITARIAMENTE</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C51" t="str">
+        <f>IF(B51&lt;&gt;"",INDEX(Inventario_Lotes!C:C,MATCH(B51,Inventario_Lotes!D:D,0)),"")</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>